<commit_message>
Update on small details
</commit_message>
<xml_diff>
--- a/Project requirements.xlsx
+++ b/Project requirements.xlsx
@@ -96,9 +96,6 @@
     <t>The application should contain a GUI</t>
   </si>
   <si>
-    <t>if the message fails to send due to an error, the system should prompt the recipient by sending an error message.</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
@@ -109,15 +106,25 @@
   </si>
   <si>
     <t>Normal user should be able to change, add mails and keywords registered in the database</t>
+  </si>
+  <si>
+    <t>If the message fails to send due to an error, the system should prompt the recipient by sending an error message.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -172,28 +179,28 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -466,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,7 +484,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,14 +694,14 @@
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>24</v>
+      <c r="B15" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>6</v>
@@ -704,8 +711,8 @@
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>26</v>
+      <c r="B16" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>21</v>
@@ -721,14 +728,14 @@
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>27</v>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>18</v>
@@ -739,13 +746,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>6</v>

</xml_diff>